<commit_message>
tile extraction, cell segmentation
</commit_message>
<xml_diff>
--- a/Labels/filered_final_labels_wsi.xlsx
+++ b/Labels/filered_final_labels_wsi.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,11 +441,6 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>F/U</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
           <t>NMYC</t>
         </is>
       </c>
@@ -456,8 +451,7 @@
           <t>DI-MH-694-08</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr">
+      <c r="B2" t="inlineStr">
         <is>
           <t>p</t>
         </is>
@@ -469,8 +463,7 @@
           <t>DI-MH-694-09</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr">
+      <c r="B3" t="inlineStr">
         <is>
           <t>p</t>
         </is>
@@ -484,11 +477,6 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
           <t>p</t>
         </is>
       </c>
@@ -501,11 +489,6 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>U</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
           <t>p</t>
         </is>
       </c>
@@ -518,11 +501,6 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
           <t>n</t>
         </is>
       </c>
@@ -535,11 +513,6 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>U</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
           <t>n</t>
         </is>
       </c>
@@ -552,11 +525,6 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>U</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
           <t>p</t>
         </is>
       </c>
@@ -569,11 +537,6 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
           <t>n</t>
         </is>
       </c>
@@ -586,11 +549,6 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
           <t>n</t>
         </is>
       </c>
@@ -601,8 +559,7 @@
           <t>DI-MH-226-06</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr"/>
-      <c r="C11" t="inlineStr">
+      <c r="B11" t="inlineStr">
         <is>
           <t>n</t>
         </is>
@@ -616,11 +573,6 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>U</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
           <t>p</t>
         </is>
       </c>
@@ -633,11 +585,6 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>U</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
           <t>p</t>
         </is>
       </c>
@@ -650,11 +597,6 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
           <t>n</t>
         </is>
       </c>
@@ -667,11 +609,6 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
           <t>n</t>
         </is>
       </c>
@@ -684,11 +621,6 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
           <t>n</t>
         </is>
       </c>
@@ -701,11 +633,6 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>U</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
           <t>n</t>
         </is>
       </c>
@@ -718,11 +645,6 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
           <t>n</t>
         </is>
       </c>
@@ -735,11 +657,6 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>U</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
           <t>n</t>
         </is>
       </c>
@@ -752,11 +669,6 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
           <t>n</t>
         </is>
       </c>
@@ -769,11 +681,6 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>U</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
           <t>n</t>
         </is>
       </c>
@@ -786,11 +693,6 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
           <t>n</t>
         </is>
       </c>
@@ -801,8 +703,7 @@
           <t>DI-MH-694-01</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr"/>
-      <c r="C23" t="inlineStr">
+      <c r="B23" t="inlineStr">
         <is>
           <t>p</t>
         </is>
@@ -814,8 +715,7 @@
           <t>DI-MH-694-04</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr"/>
-      <c r="C24" t="inlineStr">
+      <c r="B24" t="inlineStr">
         <is>
           <t>p</t>
         </is>
@@ -827,8 +727,7 @@
           <t>1</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr"/>
-      <c r="C25" t="inlineStr">
+      <c r="B25" t="inlineStr">
         <is>
           <t>p</t>
         </is>
@@ -840,8 +739,7 @@
           <t>2</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr"/>
-      <c r="C26" t="inlineStr">
+      <c r="B26" t="inlineStr">
         <is>
           <t>p</t>
         </is>
@@ -853,8 +751,7 @@
           <t>3</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr"/>
-      <c r="C27" t="inlineStr">
+      <c r="B27" t="inlineStr">
         <is>
           <t>p</t>
         </is>
@@ -866,8 +763,7 @@
           <t>4</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr"/>
-      <c r="C28" t="inlineStr">
+      <c r="B28" t="inlineStr">
         <is>
           <t>p</t>
         </is>
@@ -879,8 +775,7 @@
           <t>5</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr"/>
-      <c r="C29" t="inlineStr">
+      <c r="B29" t="inlineStr">
         <is>
           <t>p</t>
         </is>
@@ -892,8 +787,7 @@
           <t>6</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr"/>
-      <c r="C30" t="inlineStr">
+      <c r="B30" t="inlineStr">
         <is>
           <t>p</t>
         </is>
@@ -905,8 +799,7 @@
           <t>7</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr"/>
-      <c r="C31" t="inlineStr">
+      <c r="B31" t="inlineStr">
         <is>
           <t>p</t>
         </is>

</xml_diff>

<commit_message>
cell segmentation using yolo, cancer cell classification model training
</commit_message>
<xml_diff>
--- a/Labels/filered_final_labels_wsi.xlsx
+++ b/Labels/filered_final_labels_wsi.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>